<commit_message>
new daftar lalulintas UAT
</commit_message>
<xml_diff>
--- a/Filexel/KeamananUAT.xlsx
+++ b/Filexel/KeamananUAT.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="17540" activeTab="1"/>
+    <workbookView windowWidth="28000" windowHeight="15960" firstSheet="17" activeTab="21"/>
   </bookViews>
   <sheets>
     <sheet name="DaftarLaluLintas_Input" sheetId="1" r:id="rId1"/>
@@ -27,13 +27,15 @@
     <sheet name="EditManajemenPenghuniBaru" sheetId="22" r:id="rId18"/>
     <sheet name="tambahBlokdanKamar" sheetId="17" r:id="rId19"/>
     <sheet name="editBlokdanKamar" sheetId="19" r:id="rId20"/>
+    <sheet name="ManajemenKamarIndex" sheetId="23" r:id="rId21"/>
+    <sheet name="ManajemenKamarCari" sheetId="24" r:id="rId22"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="285">
   <si>
     <t>READ BARIS</t>
   </si>
@@ -840,6 +842,54 @@
   </si>
   <si>
     <t xml:space="preserve"> edt</t>
+  </si>
+  <si>
+    <t>Namaindex</t>
+  </si>
+  <si>
+    <t>NoRegisindex</t>
+  </si>
+  <si>
+    <t>SemuaIndex</t>
+  </si>
+  <si>
+    <t>StatusIndex</t>
+  </si>
+  <si>
+    <t>namaIndex</t>
+  </si>
+  <si>
+    <t>noregisIndex</t>
+  </si>
+  <si>
+    <t>CAH BIN A</t>
+  </si>
+  <si>
+    <t>Ditolak</t>
+  </si>
+  <si>
+    <t>filterColumnCari</t>
+  </si>
+  <si>
+    <t>NamaCari</t>
+  </si>
+  <si>
+    <t>NoRegisCari</t>
+  </si>
+  <si>
+    <t>SemuaCari</t>
+  </si>
+  <si>
+    <t>KejahatanCari</t>
+  </si>
+  <si>
+    <t>namaCari</t>
+  </si>
+  <si>
+    <t>noregisCari</t>
+  </si>
+  <si>
+    <t>semuaCari</t>
   </si>
 </sst>
 </file>
@@ -848,9 +898,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -861,16 +911,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10.5"/>
+      <color rgb="FF606266"/>
+      <name val="Roboto"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="10.5"/>
-      <color rgb="FF606266"/>
-      <name val="Roboto"/>
       <charset val="134"/>
     </font>
     <font>
@@ -890,14 +940,52 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -913,9 +1001,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -929,69 +1024,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1006,14 +1041,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1027,8 +1062,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1043,13 +1093,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1091,13 +1147,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="1" tint="0.5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="1" tint="0.5"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1109,19 +1177,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1139,6 +1213,30 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1151,61 +1249,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1223,25 +1285,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1253,19 +1303,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1601,6 +1651,32 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -1612,21 +1688,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1648,20 +1709,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1684,8 +1734,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1693,163 +1743,166 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="30" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="26" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="23" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="29" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="26" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="25" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="30" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="29" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="24" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1858,73 +1911,73 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2276,262 +2329,262 @@
   <dimension ref="A1:H49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="14.0078125" style="51" customWidth="1"/>
-    <col min="2" max="2" width="27.46875" style="51" customWidth="1"/>
-    <col min="3" max="3" width="30.203125" style="51" customWidth="1"/>
-    <col min="4" max="4" width="16.859375" style="52" customWidth="1"/>
-    <col min="5" max="5" width="21.4296875" style="52" customWidth="1"/>
-    <col min="6" max="6" width="23.6875" style="51" customWidth="1"/>
+    <col min="1" max="1" width="14.0078125" style="54" customWidth="1"/>
+    <col min="2" max="2" width="27.46875" style="54" customWidth="1"/>
+    <col min="3" max="3" width="30.203125" style="54" customWidth="1"/>
+    <col min="4" max="4" width="16.859375" style="55" customWidth="1"/>
+    <col min="5" max="5" width="21.4296875" style="55" customWidth="1"/>
+    <col min="6" max="6" width="23.6875" style="54" customWidth="1"/>
     <col min="7" max="7" width="14.96875" customWidth="1"/>
     <col min="8" max="8" width="26.953125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="19.5" customHeight="1" spans="1:8">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="33" t="s">
+      <c r="C1" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="59" t="s">
+      <c r="D1" s="62" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="59" t="s">
+      <c r="E1" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="63" t="s">
+      <c r="F1" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="33" t="s">
+      <c r="G1" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="36" t="s">
+      <c r="H1" s="39" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" ht="19.5" customHeight="1" spans="1:8">
-      <c r="A2" s="60">
+      <c r="A2" s="63">
         <v>3</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="57" t="s">
+      <c r="C2" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="30" t="s">
+      <c r="D2" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="30" t="s">
+      <c r="E2" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="H2" s="17" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" ht="19.5" customHeight="1" spans="1:8">
-      <c r="A3" s="34"/>
-      <c r="B3" s="8" t="s">
+      <c r="A3" s="37"/>
+      <c r="B3" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="57" t="s">
+      <c r="C3" s="60" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="30" t="s">
+      <c r="D3" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="30" t="s">
+      <c r="E3" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="H3" s="17" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="34"/>
-      <c r="B4" s="8" t="s">
+      <c r="A4" s="37"/>
+      <c r="B4" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="57" t="s">
+      <c r="C4" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="30" t="s">
+      <c r="D4" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="30" t="s">
+      <c r="E4" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="14" t="s">
+      <c r="H4" s="17" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="34"/>
-      <c r="B5" s="8" t="s">
+      <c r="A5" s="37"/>
+      <c r="B5" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="57" t="s">
+      <c r="C5" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="30" t="s">
+      <c r="D5" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="30" t="s">
+      <c r="E5" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="14" t="s">
+      <c r="H5" s="17" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="34"/>
-      <c r="B6" s="8" t="s">
+      <c r="A6" s="37"/>
+      <c r="B6" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="57" t="s">
+      <c r="C6" s="60" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="30" t="s">
+      <c r="D6" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="30" t="s">
+      <c r="E6" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="G6" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="H6" s="14" t="s">
+      <c r="H6" s="17" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="34"/>
-      <c r="B7" s="8" t="s">
+      <c r="A7" s="37"/>
+      <c r="B7" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="57" t="s">
+      <c r="C7" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="30" t="s">
+      <c r="D7" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="30" t="s">
+      <c r="E7" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="F7" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="G7" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="14" t="s">
+      <c r="H7" s="17" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="34"/>
-      <c r="B8" s="8" t="s">
+      <c r="A8" s="37"/>
+      <c r="B8" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="57" t="s">
+      <c r="C8" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="30" t="s">
+      <c r="D8" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="30" t="s">
+      <c r="E8" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="F8" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="8" t="s">
+      <c r="G8" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="H8" s="14" t="s">
+      <c r="H8" s="17" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="34"/>
-      <c r="B9" s="8" t="s">
+      <c r="A9" s="37"/>
+      <c r="B9" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="57" t="s">
+      <c r="C9" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="30" t="s">
+      <c r="D9" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="30" t="s">
+      <c r="E9" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="F9" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="G9" s="8" t="s">
+      <c r="G9" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="H9" s="14" t="s">
+      <c r="H9" s="17" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="10" ht="14.75" spans="1:8">
-      <c r="A10" s="35"/>
-      <c r="B10" s="10" t="s">
+      <c r="A10" s="38"/>
+      <c r="B10" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="57" t="s">
+      <c r="C10" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="61" t="s">
+      <c r="D10" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="61" t="s">
+      <c r="E10" s="64" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="F10" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="G10" s="10" t="s">
+      <c r="G10" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="H10" s="37" t="s">
+      <c r="H10" s="40" t="s">
         <v>13</v>
       </c>
     </row>
@@ -2611,7 +2664,7 @@
       <c r="A20"/>
       <c r="B20"/>
       <c r="C20"/>
-      <c r="D20" s="62"/>
+      <c r="D20" s="65"/>
       <c r="E20"/>
       <c r="F20"/>
     </row>
@@ -2619,7 +2672,7 @@
       <c r="A21"/>
       <c r="B21"/>
       <c r="C21"/>
-      <c r="D21" s="62"/>
+      <c r="D21" s="65"/>
       <c r="E21"/>
       <c r="F21"/>
     </row>
@@ -2627,7 +2680,7 @@
       <c r="A22"/>
       <c r="B22"/>
       <c r="C22"/>
-      <c r="D22" s="62"/>
+      <c r="D22" s="65"/>
       <c r="E22"/>
       <c r="F22"/>
     </row>
@@ -2635,7 +2688,7 @@
       <c r="A23"/>
       <c r="B23"/>
       <c r="C23"/>
-      <c r="D23" s="62"/>
+      <c r="D23" s="65"/>
       <c r="E23"/>
       <c r="F23"/>
     </row>
@@ -2643,7 +2696,7 @@
       <c r="A24"/>
       <c r="B24"/>
       <c r="C24"/>
-      <c r="D24" s="62"/>
+      <c r="D24" s="65"/>
       <c r="E24"/>
       <c r="F24"/>
     </row>
@@ -2651,7 +2704,7 @@
       <c r="A25"/>
       <c r="B25"/>
       <c r="C25"/>
-      <c r="D25" s="62"/>
+      <c r="D25" s="65"/>
       <c r="E25"/>
       <c r="F25"/>
     </row>
@@ -2659,7 +2712,7 @@
       <c r="A26"/>
       <c r="B26"/>
       <c r="C26"/>
-      <c r="D26" s="62"/>
+      <c r="D26" s="65"/>
       <c r="E26"/>
       <c r="F26"/>
     </row>
@@ -2667,7 +2720,7 @@
       <c r="A27"/>
       <c r="B27"/>
       <c r="C27"/>
-      <c r="D27" s="62"/>
+      <c r="D27" s="65"/>
       <c r="E27"/>
       <c r="F27"/>
     </row>
@@ -2675,7 +2728,7 @@
       <c r="A28"/>
       <c r="B28"/>
       <c r="C28"/>
-      <c r="D28" s="62"/>
+      <c r="D28" s="65"/>
       <c r="E28"/>
       <c r="F28"/>
     </row>
@@ -3395,126 +3448,126 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:9">
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="35" t="s">
         <v>162</v>
       </c>
-      <c r="C1" s="33" t="s">
+      <c r="C1" s="36" t="s">
         <v>163</v>
       </c>
-      <c r="D1" s="33" t="s">
+      <c r="D1" s="36" t="s">
         <v>164</v>
       </c>
-      <c r="E1" s="33" t="s">
+      <c r="E1" s="36" t="s">
         <v>165</v>
       </c>
-      <c r="F1" s="33" t="s">
+      <c r="F1" s="36" t="s">
         <v>166</v>
       </c>
-      <c r="G1" s="33" t="s">
+      <c r="G1" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="H1" s="33" t="s">
+      <c r="H1" s="36" t="s">
         <v>167</v>
       </c>
-      <c r="I1" s="36" t="s">
+      <c r="I1" s="39" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="2" spans="2:9">
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="37" t="s">
         <v>164</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="11" t="s">
         <v>168</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="11" t="s">
         <v>169</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="11" t="s">
         <v>170</v>
       </c>
-      <c r="F2" s="8">
+      <c r="F2" s="11">
         <v>2</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="11" t="s">
         <v>171</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="11" t="s">
         <v>172</v>
       </c>
-      <c r="I2" s="14" t="s">
+      <c r="I2" s="17" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="3" spans="2:9">
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="37" t="s">
         <v>174</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="11" t="s">
         <v>176</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="11" t="s">
         <v>177</v>
       </c>
-      <c r="F3" s="8">
+      <c r="F3" s="11">
         <v>1</v>
       </c>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8" t="s">
+      <c r="G3" s="11"/>
+      <c r="H3" s="11" t="s">
         <v>172</v>
       </c>
-      <c r="I3" s="14" t="s">
+      <c r="I3" s="17" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="4" spans="2:9">
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="37" t="s">
         <v>166</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="11" t="s">
         <v>178</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="11" t="s">
         <v>169</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="11" t="s">
         <v>179</v>
       </c>
-      <c r="F4" s="8">
+      <c r="F4" s="11">
         <v>3</v>
       </c>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8" t="s">
+      <c r="G4" s="11"/>
+      <c r="H4" s="11" t="s">
         <v>172</v>
       </c>
-      <c r="I4" s="14" t="s">
+      <c r="I4" s="17" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="5" ht="14.75" spans="2:9">
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="38" t="s">
         <v>165</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="13" t="s">
         <v>180</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="13" t="s">
         <v>176</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="13" t="s">
         <v>170</v>
       </c>
-      <c r="F5" s="10">
+      <c r="F5" s="13">
         <v>1</v>
       </c>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10" t="s">
+      <c r="G5" s="13"/>
+      <c r="H5" s="13" t="s">
         <v>172</v>
       </c>
-      <c r="I5" s="37" t="s">
+      <c r="I5" s="40" t="s">
         <v>173</v>
       </c>
     </row>
@@ -3611,7 +3664,7 @@
       <c r="I2" t="s">
         <v>193</v>
       </c>
-      <c r="J2" s="30" t="s">
+      <c r="J2" s="33" t="s">
         <v>10</v>
       </c>
       <c r="K2" t="s">
@@ -3643,7 +3696,7 @@
       <c r="I3" t="s">
         <v>198</v>
       </c>
-      <c r="J3" s="30" t="s">
+      <c r="J3" s="33" t="s">
         <v>199</v>
       </c>
       <c r="K3" t="s">
@@ -3675,7 +3728,7 @@
       <c r="I4" t="s">
         <v>201</v>
       </c>
-      <c r="J4" s="30" t="s">
+      <c r="J4" s="33" t="s">
         <v>202</v>
       </c>
       <c r="K4" t="s">
@@ -3707,7 +3760,7 @@
       <c r="I5" t="s">
         <v>203</v>
       </c>
-      <c r="J5" s="30" t="s">
+      <c r="J5" s="33" t="s">
         <v>204</v>
       </c>
       <c r="K5" t="s">
@@ -3745,147 +3798,147 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:10">
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="31" t="s">
         <v>162</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="31" t="s">
         <v>205</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="D1" s="31" t="s">
         <v>206</v>
       </c>
-      <c r="E1" s="28" t="s">
+      <c r="E1" s="31" t="s">
         <v>174</v>
       </c>
-      <c r="F1" s="28" t="s">
+      <c r="F1" s="31" t="s">
         <v>207</v>
       </c>
-      <c r="G1" s="28" t="s">
+      <c r="G1" s="31" t="s">
         <v>208</v>
       </c>
-      <c r="H1" s="28" t="s">
+      <c r="H1" s="31" t="s">
         <v>209</v>
       </c>
-      <c r="I1" s="31" t="s">
+      <c r="I1" s="34" t="s">
         <v>167</v>
       </c>
-      <c r="J1" s="28" t="s">
+      <c r="J1" s="31" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="2" spans="2:10">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="11" t="s">
         <v>210</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="D2" s="8">
+      <c r="D2" s="11">
         <v>0</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="11" t="s">
         <v>169</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="11" t="s">
         <v>211</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="I2" s="11" t="s">
         <v>172</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="J2" s="11" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="3" spans="2:10">
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="11">
         <v>0</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="11" t="s">
         <v>176</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="H3" s="11" t="s">
         <v>213</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="I3" s="11" t="s">
         <v>172</v>
       </c>
-      <c r="J3" s="8" t="s">
+      <c r="J3" s="11" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="4" spans="2:10">
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="11" t="s">
         <v>214</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="11">
         <v>0</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="11" t="s">
         <v>169</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="H4" s="11" t="s">
         <v>211</v>
       </c>
-      <c r="I4" s="8" t="s">
+      <c r="I4" s="11" t="s">
         <v>172</v>
       </c>
-      <c r="J4" s="8" t="s">
+      <c r="J4" s="11" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="5" ht="14.75" spans="2:10">
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="11" t="s">
         <v>187</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="11">
         <v>0</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="11" t="s">
         <v>176</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="H5" s="11" t="s">
         <v>213</v>
       </c>
-      <c r="I5" s="10" t="s">
+      <c r="I5" s="13" t="s">
         <v>172</v>
       </c>
-      <c r="J5" s="8" t="s">
+      <c r="J5" s="11" t="s">
         <v>212</v>
       </c>
     </row>
@@ -3931,162 +3984,162 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11">
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="31" t="s">
         <v>215</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="D1" s="31" t="s">
         <v>216</v>
       </c>
-      <c r="E1" s="28" t="s">
+      <c r="E1" s="31" t="s">
         <v>217</v>
       </c>
-      <c r="F1" s="28" t="s">
+      <c r="F1" s="31" t="s">
         <v>210</v>
       </c>
-      <c r="G1" s="28" t="s">
+      <c r="G1" s="31" t="s">
         <v>218</v>
       </c>
-      <c r="H1" s="28" t="s">
+      <c r="H1" s="31" t="s">
         <v>219</v>
       </c>
-      <c r="I1" s="28" t="s">
+      <c r="I1" s="31" t="s">
         <v>220</v>
       </c>
-      <c r="J1" s="28" t="s">
+      <c r="J1" s="31" t="s">
         <v>221</v>
       </c>
-      <c r="K1" s="28" t="s">
+      <c r="K1" s="31" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="2" spans="2:11">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="11" t="s">
         <v>210</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="D2" s="8">
+      <c r="D2" s="11">
         <v>0</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="11" t="s">
         <v>169</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="11" t="s">
         <v>191</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="11" t="s">
         <v>192</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="I2" s="11" t="s">
         <v>193</v>
       </c>
-      <c r="J2" s="30" t="s">
+      <c r="J2" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="K2" s="11" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="3" spans="2:11">
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="11" t="s">
         <v>210</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="11" t="s">
         <v>196</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="11">
         <v>0</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="11" t="s">
         <v>176</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="11" t="s">
         <v>197</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="H3" s="11" t="s">
         <v>192</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="I3" s="11" t="s">
         <v>198</v>
       </c>
-      <c r="J3" s="30" t="s">
+      <c r="J3" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="K3" s="8" t="s">
+      <c r="K3" s="11" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="4" spans="2:11">
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="11" t="s">
         <v>210</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="11" t="s">
         <v>200</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="11">
         <v>0</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="11" t="s">
         <v>169</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="11" t="s">
         <v>191</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="H4" s="11" t="s">
         <v>192</v>
       </c>
-      <c r="I4" s="8" t="s">
+      <c r="I4" s="11" t="s">
         <v>201</v>
       </c>
-      <c r="J4" s="30" t="s">
+      <c r="J4" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="K4" s="8" t="s">
+      <c r="K4" s="11" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="5" spans="2:11">
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="11" t="s">
         <v>210</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="11">
         <v>0</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="11" t="s">
         <v>176</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="11" t="s">
         <v>191</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="H5" s="11" t="s">
         <v>192</v>
       </c>
-      <c r="I5" s="8" t="s">
+      <c r="I5" s="11" t="s">
         <v>203</v>
       </c>
-      <c r="J5" s="30" t="s">
+      <c r="J5" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="K5" s="8" t="s">
+      <c r="K5" s="11" t="s">
         <v>194</v>
       </c>
     </row>
@@ -4135,288 +4188,288 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="11" t="s">
         <v>223</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8" t="s">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11" t="s">
         <v>224</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="11" t="s">
         <v>165</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="11" t="s">
         <v>225</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="11" t="s">
         <v>226</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="11" t="s">
         <v>227</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="11" t="s">
         <v>228</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="11" t="s">
         <v>229</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="11" t="s">
         <v>230</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="L1" s="11" t="s">
         <v>231</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="M1" s="11" t="s">
         <v>232</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="N1" s="11" t="s">
         <v>233</v>
       </c>
-      <c r="O1" s="8" t="s">
+      <c r="O1" s="11" t="s">
         <v>234</v>
       </c>
-      <c r="P1" s="8" t="s">
+      <c r="P1" s="11" t="s">
         <v>235</v>
       </c>
-      <c r="Q1" s="8" t="s">
+      <c r="Q1" s="11" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="2" spans="1:17">
-      <c r="A2" s="8">
+      <c r="A2" s="11">
         <v>1</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8" t="s">
+      <c r="B2" s="11"/>
+      <c r="C2" s="11" t="s">
         <v>237</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="11" t="s">
         <v>170</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="11" t="s">
         <v>238</v>
       </c>
-      <c r="F2" s="28" t="s">
+      <c r="F2" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="G2" s="29">
+      <c r="G2" s="32">
         <v>2</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="11" t="s">
         <v>239</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="I2" s="11" t="s">
         <v>240</v>
       </c>
-      <c r="J2" s="8">
+      <c r="J2" s="11">
         <v>10</v>
       </c>
-      <c r="K2" s="8">
+      <c r="K2" s="11">
         <v>1</v>
       </c>
-      <c r="L2" s="8">
+      <c r="L2" s="11">
         <v>10</v>
       </c>
-      <c r="M2" s="8" t="s">
+      <c r="M2" s="11" t="s">
         <v>241</v>
       </c>
-      <c r="N2" s="28" t="s">
+      <c r="N2" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="O2" s="8">
+      <c r="O2" s="11">
         <v>30</v>
       </c>
-      <c r="P2" s="8" t="s">
+      <c r="P2" s="11" t="s">
         <v>242</v>
       </c>
-      <c r="Q2" s="8">
+      <c r="Q2" s="11">
         <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:17">
-      <c r="A3" s="8">
+      <c r="A3" s="11">
         <v>2</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8" t="s">
+      <c r="B3" s="11"/>
+      <c r="C3" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="11" t="s">
         <v>179</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="11" t="s">
         <v>238</v>
       </c>
-      <c r="F3" s="28" t="s">
+      <c r="F3" s="31" t="s">
         <v>243</v>
       </c>
-      <c r="G3" s="29">
+      <c r="G3" s="32">
         <v>1</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="H3" s="11" t="s">
         <v>244</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="I3" s="11" t="s">
         <v>245</v>
       </c>
-      <c r="J3" s="8">
+      <c r="J3" s="11">
         <v>15</v>
       </c>
-      <c r="K3" s="8">
+      <c r="K3" s="11">
         <v>2</v>
       </c>
-      <c r="L3" s="8">
+      <c r="L3" s="11">
         <v>15</v>
       </c>
-      <c r="M3" s="8" t="s">
+      <c r="M3" s="11" t="s">
         <v>246</v>
       </c>
-      <c r="N3" s="28" t="s">
+      <c r="N3" s="31" t="s">
         <v>243</v>
       </c>
-      <c r="O3" s="8">
+      <c r="O3" s="11">
         <v>33</v>
       </c>
-      <c r="P3" s="8" t="s">
+      <c r="P3" s="11" t="s">
         <v>247</v>
       </c>
-      <c r="Q3" s="8">
+      <c r="Q3" s="11">
         <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:17">
-      <c r="A4" s="8">
+      <c r="A4" s="11">
         <v>3</v>
       </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8" t="s">
+      <c r="B4" s="11"/>
+      <c r="C4" s="11" t="s">
         <v>248</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="11" t="s">
         <v>249</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="11" t="s">
         <v>238</v>
       </c>
-      <c r="F4" s="28" t="s">
+      <c r="F4" s="31" t="s">
         <v>250</v>
       </c>
-      <c r="G4" s="29">
+      <c r="G4" s="32">
         <v>3</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="H4" s="11" t="s">
         <v>251</v>
       </c>
-      <c r="I4" s="8" t="s">
+      <c r="I4" s="11" t="s">
         <v>252</v>
       </c>
-      <c r="J4" s="8">
+      <c r="J4" s="11">
         <v>14</v>
       </c>
-      <c r="K4" s="8">
+      <c r="K4" s="11">
         <v>3</v>
       </c>
-      <c r="L4" s="8">
+      <c r="L4" s="11">
         <v>14</v>
       </c>
-      <c r="M4" s="8" t="s">
+      <c r="M4" s="11" t="s">
         <v>253</v>
       </c>
-      <c r="N4" s="28" t="s">
+      <c r="N4" s="31" t="s">
         <v>250</v>
       </c>
-      <c r="O4" s="8">
+      <c r="O4" s="11">
         <v>43</v>
       </c>
-      <c r="P4" s="8" t="s">
+      <c r="P4" s="11" t="s">
         <v>242</v>
       </c>
-      <c r="Q4" s="8">
+      <c r="Q4" s="11">
         <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:17">
-      <c r="A5" s="8">
+      <c r="A5" s="11">
         <v>4</v>
       </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8" t="s">
+      <c r="B5" s="11"/>
+      <c r="C5" s="11" t="s">
         <v>191</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="11" t="s">
         <v>170</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="11" t="s">
         <v>254</v>
       </c>
-      <c r="F5" s="28" t="s">
+      <c r="F5" s="31" t="s">
         <v>255</v>
       </c>
-      <c r="G5" s="29">
+      <c r="G5" s="32">
         <v>2</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="H5" s="11" t="s">
         <v>256</v>
       </c>
-      <c r="I5" s="8" t="s">
+      <c r="I5" s="11" t="s">
         <v>240</v>
       </c>
-      <c r="J5" s="8">
+      <c r="J5" s="11">
         <v>12</v>
       </c>
-      <c r="K5" s="8">
+      <c r="K5" s="11">
         <v>4</v>
       </c>
-      <c r="L5" s="8">
+      <c r="L5" s="11">
         <v>12</v>
       </c>
-      <c r="M5" s="8" t="s">
+      <c r="M5" s="11" t="s">
         <v>257</v>
       </c>
-      <c r="N5" s="28" t="s">
+      <c r="N5" s="31" t="s">
         <v>250</v>
       </c>
-      <c r="O5" s="8">
+      <c r="O5" s="11">
         <v>23</v>
       </c>
-      <c r="P5" s="8" t="s">
+      <c r="P5" s="11" t="s">
         <v>247</v>
       </c>
-      <c r="Q5" s="8">
+      <c r="Q5" s="11">
         <v>20</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="9">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2:P5">
+      <formula1>"Baik,Rusak"</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2:N5">
       <formula1>"Teroris,Korupsi,Narkotik,Kriminal"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H8:H12">
+      <formula1>"Angka 8 (mulai kiri atas),Angka 8 (mulai kiri bawah),Angka 8 (mulai kanani atas),Angka 8 (mulai kanan bawah),Belakang Ke Depan (1 arah),Belakang Ke Depan (2 arah),Depan Ke Belakang (1 arah),Depan Ke Belakang (2 arah),Kanan Kiri (1 arah)"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H7">
+      <formula1>"Angka 8 mulai kiri atas,Angka 8 mulai kiri bawah,Angka 8 mulai kanani atas,Angka 8 mulai kanan bawah,Belakang Ke Depan 1 arah,Belakang Ke Depan 2 arah,Depan Ke Belakang 1 arah,Depan Ke Belakang 2 arah,Kanan Kiri 1 arah"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G5">
+      <formula1>"1,2,3,4"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I9">
       <formula1>"Anak-anak,Dewasa,Lansia"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D10">
-      <formula1>"Umum,Mapenaling,Tutup Sunyi,Isolasi"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H7">
-      <formula1>"Angka 8 mulai kiri atas,Angka 8 mulai kiri bawah,Angka 8 mulai kanani atas,Angka 8 mulai kanan bawah,Belakang Ke Depan 1 arah,Belakang Ke Depan 2 arah,Depan Ke Belakang 1 arah,Depan Ke Belakang 2 arah,Kanan Kiri 1 arah"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E5">
+      <formula1>"Laki-laki,Perempuan"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F5">
       <formula1>"Korupsi,Teroris,Kriminal,Kriminal Teroris Korupsi,Korupsi Teroris,Teroris Kriminal"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G5">
-      <formula1>"1,2,3,4"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2:P5">
-      <formula1>"Baik,Rusak"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H8:H12">
-      <formula1>"Angka 8 (mulai kiri atas),Angka 8 (mulai kiri bawah),Angka 8 (mulai kanani atas),Angka 8 (mulai kanan bawah),Belakang Ke Depan (1 arah),Belakang Ke Depan (2 arah),Depan Ke Belakang (1 arah),Depan Ke Belakang (2 arah),Kanan Kiri (1 arah)"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E5">
-      <formula1>"Laki-laki,Perempuan"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D10">
+      <formula1>"Umum,Mapenaling,Tutup Sunyi,Isolasi"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4431,294 +4484,294 @@
   </sheetPr>
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="14.1484375" style="51" customWidth="1"/>
-    <col min="2" max="2" width="32.1484375" style="51" customWidth="1"/>
-    <col min="3" max="3" width="29.859375" style="51" customWidth="1"/>
-    <col min="4" max="4" width="27.1484375" style="52" customWidth="1"/>
-    <col min="5" max="5" width="32.4296875" style="52" customWidth="1"/>
-    <col min="6" max="6" width="42.0078125" style="51" customWidth="1"/>
+    <col min="1" max="1" width="14.1484375" style="54" customWidth="1"/>
+    <col min="2" max="2" width="32.1484375" style="54" customWidth="1"/>
+    <col min="3" max="3" width="29.859375" style="54" customWidth="1"/>
+    <col min="4" max="4" width="27.1484375" style="55" customWidth="1"/>
+    <col min="5" max="5" width="32.4296875" style="55" customWidth="1"/>
+    <col min="6" max="6" width="42.0078125" style="54" customWidth="1"/>
     <col min="7" max="7" width="23.703125" customWidth="1"/>
     <col min="8" max="8" width="24.8671875" customWidth="1"/>
     <col min="9" max="9" width="29.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="19.5" customHeight="1" spans="1:9">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="53" t="s">
+      <c r="B1" s="56" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="54" t="s">
+      <c r="C1" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="55" t="s">
+      <c r="D1" s="58" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="58" t="s">
+      <c r="E1" s="61" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="58" t="s">
+      <c r="F1" s="61" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="54" t="s">
+      <c r="G1" s="57" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="28" t="s">
+      <c r="H1" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="I1" s="28" t="s">
+      <c r="I1" s="31" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="2" ht="19.5" customHeight="1" spans="1:9">
-      <c r="A2" s="56">
+      <c r="A2" s="59">
         <v>3</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="57" t="s">
+      <c r="C2" s="60" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="57" t="s">
+      <c r="D2" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="30" t="s">
+      <c r="E2" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="30" t="s">
+      <c r="F2" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="I2" s="11" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" ht="19.5" customHeight="1" spans="1:9">
-      <c r="A3" s="8"/>
-      <c r="B3" s="8" t="s">
+      <c r="A3" s="11"/>
+      <c r="B3" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="57" t="s">
+      <c r="C3" s="60" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="57" t="s">
+      <c r="D3" s="60" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="30" t="s">
+      <c r="E3" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="30" t="s">
+      <c r="F3" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="H3" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="I3" s="11" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="8"/>
-      <c r="B4" s="8" t="s">
+      <c r="A4" s="11"/>
+      <c r="B4" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="57" t="s">
+      <c r="C4" s="60" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="57" t="s">
+      <c r="D4" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="30" t="s">
+      <c r="E4" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="30" t="s">
+      <c r="F4" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="H4" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="I4" s="8" t="s">
+      <c r="I4" s="11" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="8"/>
-      <c r="B5" s="8" t="s">
+      <c r="A5" s="11"/>
+      <c r="B5" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="57" t="s">
+      <c r="C5" s="60" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="57" t="s">
+      <c r="D5" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="30" t="s">
+      <c r="E5" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="30" t="s">
+      <c r="F5" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="H5" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="I5" s="8" t="s">
+      <c r="I5" s="11" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="8"/>
-      <c r="B6" s="8" t="s">
+      <c r="A6" s="11"/>
+      <c r="B6" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="57" t="s">
+      <c r="C6" s="60" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="57" t="s">
+      <c r="D6" s="60" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="30" t="s">
+      <c r="E6" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="30" t="s">
+      <c r="F6" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="G6" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="H6" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="I6" s="8" t="s">
+      <c r="I6" s="11" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="8"/>
-      <c r="B7" s="8" t="s">
+      <c r="A7" s="11"/>
+      <c r="B7" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="57" t="s">
+      <c r="C7" s="60" t="s">
         <v>35</v>
       </c>
-      <c r="D7" s="57" t="s">
+      <c r="D7" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="30" t="s">
+      <c r="E7" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="30" t="s">
+      <c r="F7" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="G7" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="H7" s="8" t="s">
+      <c r="H7" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="I7" s="8" t="s">
+      <c r="I7" s="11" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8" t="s">
+      <c r="A8" s="11"/>
+      <c r="B8" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="57" t="s">
+      <c r="C8" s="60" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="57" t="s">
+      <c r="D8" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="30" t="s">
+      <c r="E8" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="30" t="s">
+      <c r="F8" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="8" t="s">
+      <c r="G8" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="H8" s="8" t="s">
+      <c r="H8" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="I8" s="8" t="s">
+      <c r="I8" s="11" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8" t="s">
+      <c r="A9" s="11"/>
+      <c r="B9" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="57" t="s">
+      <c r="C9" s="60" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="57" t="s">
+      <c r="D9" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="30" t="s">
+      <c r="E9" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="30" t="s">
+      <c r="F9" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="8" t="s">
+      <c r="G9" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="H9" s="8" t="s">
+      <c r="H9" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="I9" s="8" t="s">
+      <c r="I9" s="11" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8" t="s">
+      <c r="A10" s="11"/>
+      <c r="B10" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="57" t="s">
+      <c r="C10" s="60" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="57" t="s">
+      <c r="D10" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="30" t="s">
+      <c r="E10" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="F10" s="30" t="s">
+      <c r="F10" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="G10" s="8" t="s">
+      <c r="G10" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="H10" s="8" t="s">
+      <c r="H10" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="I10" s="8" t="s">
+      <c r="I10" s="11" t="s">
         <v>13</v>
       </c>
     </row>
@@ -4738,8 +4791,8 @@
   <sheetPr/>
   <dimension ref="B1:V6"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="S33" sqref="S33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="5"/>
@@ -4767,420 +4820,417 @@
   </cols>
   <sheetData>
     <row r="1" ht="14.75" spans="2:22">
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="15" t="s">
         <v>258</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="I1" s="19" t="s">
         <v>259</v>
       </c>
-      <c r="J1" s="16" t="s">
+      <c r="J1" s="19" t="s">
         <v>260</v>
       </c>
-      <c r="K1" s="16" t="s">
+      <c r="K1" s="19" t="s">
         <v>261</v>
       </c>
-      <c r="L1" s="16" t="s">
+      <c r="L1" s="19" t="s">
         <v>262</v>
       </c>
-      <c r="M1" s="16" t="s">
+      <c r="M1" s="19" t="s">
         <v>263</v>
       </c>
-      <c r="N1" s="18" t="s">
+      <c r="N1" s="21" t="s">
         <v>264</v>
       </c>
-      <c r="O1" s="19" t="s">
+      <c r="O1" s="22" t="s">
         <v>265</v>
       </c>
-      <c r="P1" s="16" t="s">
+      <c r="P1" s="19" t="s">
         <v>266</v>
       </c>
-      <c r="Q1" s="18" t="s">
+      <c r="Q1" s="21" t="s">
         <v>267</v>
       </c>
-      <c r="R1" s="20" t="s">
+      <c r="R1" s="23" t="s">
         <v>232</v>
       </c>
-      <c r="S1" s="21" t="s">
+      <c r="S1" s="24" t="s">
         <v>233</v>
       </c>
-      <c r="T1" s="21" t="s">
+      <c r="T1" s="24" t="s">
         <v>234</v>
       </c>
-      <c r="U1" s="21" t="s">
+      <c r="U1" s="24" t="s">
         <v>235</v>
       </c>
-      <c r="V1" s="25" t="s">
+      <c r="V1" s="28" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="2" spans="2:22">
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="7" t="s">
         <v>168</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="7">
         <v>2</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="16" t="s">
         <v>171</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="6" t="s">
         <v>268</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="8" t="s">
         <v>238</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="K2" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="L2" s="5">
+      <c r="L2" s="8">
         <v>2</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="M2" s="8" t="s">
         <v>239</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="N2" s="8" t="s">
         <v>240</v>
       </c>
-      <c r="O2" s="5">
+      <c r="O2" s="8">
         <v>10</v>
       </c>
-      <c r="P2" s="5">
+      <c r="P2" s="8">
         <v>1</v>
       </c>
-      <c r="Q2" s="22">
+      <c r="Q2" s="25">
         <v>10</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="R2" s="6" t="s">
         <v>241</v>
       </c>
-      <c r="S2" s="5" t="s">
+      <c r="S2" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="T2" s="5">
+      <c r="T2" s="8">
         <v>30</v>
       </c>
-      <c r="U2" s="5" t="s">
+      <c r="U2" s="8" t="s">
         <v>242</v>
       </c>
-      <c r="V2" s="26">
+      <c r="V2" s="29">
         <v>30</v>
       </c>
     </row>
     <row r="3" spans="2:22">
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="10" t="s">
         <v>172</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="11" t="s">
         <v>177</v>
       </c>
-      <c r="F3" s="8">
+      <c r="F3" s="11">
         <v>1</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="G3" s="17" t="s">
         <v>171</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="9" t="s">
         <v>268</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="I3" s="10" t="s">
         <v>179</v>
       </c>
-      <c r="J3" s="7" t="s">
+      <c r="J3" s="10" t="s">
         <v>238</v>
       </c>
-      <c r="K3" s="7" t="s">
+      <c r="K3" s="10" t="s">
         <v>243</v>
       </c>
-      <c r="L3" s="7">
+      <c r="L3" s="10">
         <v>1</v>
       </c>
-      <c r="M3" s="7" t="s">
+      <c r="M3" s="10" t="s">
         <v>244</v>
       </c>
-      <c r="N3" s="7" t="s">
+      <c r="N3" s="10" t="s">
         <v>245</v>
       </c>
-      <c r="O3" s="7">
+      <c r="O3" s="10">
         <v>15</v>
       </c>
-      <c r="P3" s="7">
+      <c r="P3" s="10">
         <v>2</v>
       </c>
-      <c r="Q3" s="23">
+      <c r="Q3" s="26">
         <v>15</v>
       </c>
-      <c r="R3" s="6" t="s">
+      <c r="R3" s="9" t="s">
         <v>246</v>
       </c>
-      <c r="S3" s="7" t="s">
+      <c r="S3" s="10" t="s">
         <v>243</v>
       </c>
-      <c r="T3" s="7">
+      <c r="T3" s="10">
         <v>33</v>
       </c>
-      <c r="U3" s="7" t="s">
+      <c r="U3" s="10" t="s">
         <v>247</v>
       </c>
-      <c r="V3" s="27">
+      <c r="V3" s="30">
         <v>14</v>
       </c>
     </row>
     <row r="4" spans="2:22">
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="9" t="s">
         <v>165</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="11" t="s">
         <v>178</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="11" t="s">
         <v>176</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="10" t="s">
         <v>179</v>
       </c>
-      <c r="F4" s="8">
+      <c r="F4" s="11">
         <v>3</v>
       </c>
-      <c r="G4" s="14" t="s">
+      <c r="G4" s="17" t="s">
         <v>171</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="9" t="s">
         <v>268</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="I4" s="10" t="s">
         <v>249</v>
       </c>
-      <c r="J4" s="7" t="s">
+      <c r="J4" s="10" t="s">
         <v>238</v>
       </c>
-      <c r="K4" s="7" t="s">
+      <c r="K4" s="10" t="s">
         <v>250</v>
       </c>
-      <c r="L4" s="7">
+      <c r="L4" s="10">
         <v>3</v>
       </c>
-      <c r="M4" s="7" t="s">
+      <c r="M4" s="10" t="s">
         <v>251</v>
       </c>
-      <c r="N4" s="7" t="s">
+      <c r="N4" s="10" t="s">
         <v>252</v>
       </c>
-      <c r="O4" s="7">
+      <c r="O4" s="10">
         <v>14</v>
       </c>
-      <c r="P4" s="7">
+      <c r="P4" s="10">
         <v>3</v>
       </c>
-      <c r="Q4" s="23">
+      <c r="Q4" s="26">
         <v>14</v>
       </c>
-      <c r="R4" s="6" t="s">
+      <c r="R4" s="9" t="s">
         <v>253</v>
       </c>
-      <c r="S4" s="7" t="s">
+      <c r="S4" s="10" t="s">
         <v>250</v>
       </c>
-      <c r="T4" s="7">
+      <c r="T4" s="10">
         <v>43</v>
       </c>
-      <c r="U4" s="7" t="s">
+      <c r="U4" s="10" t="s">
         <v>242</v>
       </c>
-      <c r="V4" s="27">
+      <c r="V4" s="30">
         <v>23</v>
       </c>
     </row>
     <row r="5" spans="2:22">
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="9" t="s">
         <v>166</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="11" t="s">
         <v>180</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="11" t="s">
         <v>176</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="11" t="s">
         <v>170</v>
       </c>
-      <c r="F5" s="8">
+      <c r="F5" s="11">
         <v>1</v>
       </c>
-      <c r="G5" s="14" t="s">
+      <c r="G5" s="17" t="s">
         <v>171</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="H5" s="9" t="s">
         <v>268</v>
       </c>
-      <c r="I5" s="7" t="s">
+      <c r="I5" s="10" t="s">
         <v>170</v>
       </c>
-      <c r="J5" s="7" t="s">
+      <c r="J5" s="10" t="s">
         <v>254</v>
       </c>
-      <c r="K5" s="7" t="s">
+      <c r="K5" s="10" t="s">
         <v>255</v>
       </c>
-      <c r="L5" s="7">
+      <c r="L5" s="10">
         <v>2</v>
       </c>
-      <c r="M5" s="7" t="s">
+      <c r="M5" s="10" t="s">
         <v>256</v>
       </c>
-      <c r="N5" s="7" t="s">
+      <c r="N5" s="10" t="s">
         <v>240</v>
       </c>
-      <c r="O5" s="7">
+      <c r="O5" s="10">
         <v>12</v>
       </c>
-      <c r="P5" s="7">
+      <c r="P5" s="10">
         <v>4</v>
       </c>
-      <c r="Q5" s="23">
+      <c r="Q5" s="26">
         <v>12</v>
       </c>
-      <c r="R5" s="6" t="s">
+      <c r="R5" s="9" t="s">
         <v>257</v>
       </c>
-      <c r="S5" s="7" t="s">
+      <c r="S5" s="10" t="s">
         <v>250</v>
       </c>
-      <c r="T5" s="7">
+      <c r="T5" s="10">
         <v>23</v>
       </c>
-      <c r="U5" s="7" t="s">
+      <c r="U5" s="10" t="s">
         <v>247</v>
       </c>
-      <c r="V5" s="27">
+      <c r="V5" s="30">
         <v>20</v>
       </c>
     </row>
     <row r="6" ht="14.75" spans="2:22">
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="13" t="s">
         <v>180</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="13" t="s">
         <v>176</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="13" t="s">
         <v>170</v>
       </c>
-      <c r="F6" s="10">
+      <c r="F6" s="13">
         <v>1</v>
       </c>
-      <c r="G6" s="15" t="s">
+      <c r="G6" s="18" t="s">
         <v>171</v>
       </c>
-      <c r="H6" s="9" t="s">
+      <c r="H6" s="12" t="s">
         <v>268</v>
       </c>
-      <c r="I6" s="17" t="s">
+      <c r="I6" s="20" t="s">
         <v>170</v>
       </c>
-      <c r="J6" s="17" t="s">
+      <c r="J6" s="20" t="s">
         <v>254</v>
       </c>
-      <c r="K6" s="17" t="s">
+      <c r="K6" s="20" t="s">
         <v>255</v>
       </c>
-      <c r="L6" s="17">
+      <c r="L6" s="20">
         <v>2</v>
       </c>
-      <c r="M6" s="17" t="s">
+      <c r="M6" s="20" t="s">
         <v>256</v>
       </c>
-      <c r="N6" s="17" t="s">
+      <c r="N6" s="20" t="s">
         <v>240</v>
       </c>
-      <c r="O6" s="17">
+      <c r="O6" s="20">
         <v>12</v>
       </c>
-      <c r="P6" s="17">
+      <c r="P6" s="20">
         <v>5</v>
       </c>
-      <c r="Q6" s="24">
+      <c r="Q6" s="27">
         <v>15</v>
       </c>
-      <c r="R6" s="9" t="s">
+      <c r="R6" s="12" t="s">
         <v>257</v>
       </c>
-      <c r="S6" s="17" t="s">
+      <c r="S6" s="20" t="s">
         <v>250</v>
       </c>
-      <c r="T6" s="17">
+      <c r="T6" s="20">
         <v>23</v>
       </c>
-      <c r="U6" s="17" t="s">
+      <c r="U6" s="20" t="s">
         <v>247</v>
       </c>
-      <c r="V6" s="15">
+      <c r="V6" s="18">
         <v>20</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I6">
+      <formula1>"Umum,Tutup Sunyi,Mapenaling,Isolasi"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U6 U2:U5">
+      <formula1>"Baik,Rusak"</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S6 S2:S5">
       <formula1>"Teroris,Korupsi,Narkotik,Kriminal"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M6 M2:M5">
+      <formula1>"Angka 8 mulai kiri atas,Angka 8 mulai kiri bawah,Angka 8 mulai kanani atas,Angka 8 mulai kanan bawah,Belakang Ke Depan 1 arah,Belakang Ke Depan 2 arah,Depan Ke Belakang 1 arah,Depan Ke Belakang 2 arah,Kanan Kiri 1 arah"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L6 L2:L5">
+      <formula1>"1,2,3,4"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N6 N2:N5">
       <formula1>"Anak-anak,Dewasa,Lansia"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M6 M2:M5">
-      <formula1>"Angka 8 mulai kiri atas,Angka 8 mulai kiri bawah,Angka 8 mulai kanani atas,Angka 8 mulai kanan bawah,Belakang Ke Depan 1 arah,Belakang Ke Depan 2 arah,Depan Ke Belakang 1 arah,Depan Ke Belakang 2 arah,Kanan Kiri 1 arah"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I6">
-      <formula1>"Umum,Tutup Sunyi,Mapenaling,Isolasi"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L6 L2:L5">
-      <formula1>"1,2,3,4"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U6 U2:U5">
-      <formula1>"Baik,Rusak"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6 B2:B5">
-      <formula1>"status,blok,jumlahlantai,semua,tipeblok"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J6 J2:J5">
-      <formula1>"Laki-laki,Perempuan"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K6 K2:K5">
+      <formula1>"Korupsi,Teroris,Kriminal,Kriminal Teroris Korupsi,Korupsi Teroris,Teroris Kriminal"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6 E2:E5">
       <formula1>"Mapenaling,Umum,Tutup Sunyi,Isolasi"</formula1>
@@ -5188,8 +5238,249 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6 D2:D5">
       <formula1>"Diizinkan,Perbaikan,Dalam Proses"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K6 K2:K5">
-      <formula1>"Korupsi,Teroris,Kriminal,Kriminal Teroris Korupsi,Korupsi Teroris,Teroris Kriminal"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J6 J2:J5">
+      <formula1>"Laki-laki,Perempuan"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6 B2:B5">
+      <formula1>"status,blok,jumlahlantai,semua,tipeblok"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="B1:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="5" outlineLevelCol="5"/>
+  <cols>
+    <col min="2" max="2" width="19.78125" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="19.0078125" customWidth="1"/>
+    <col min="5" max="5" width="19.2734375" customWidth="1"/>
+    <col min="6" max="6" width="20.96875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:6">
+      <c r="B1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="2" spans="2:6">
+      <c r="B2" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="3" ht="15.6" spans="2:6">
+      <c r="B3" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>83</v>
+      </c>
+      <c r="F3" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="4" ht="15.6" spans="2:6">
+      <c r="B4" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>83</v>
+      </c>
+      <c r="F4" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6">
+      <c r="B5" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>83</v>
+      </c>
+      <c r="F5" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="6" spans="4:6">
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>83</v>
+      </c>
+      <c r="F6" t="s">
+        <v>183</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F6">
+      <formula1>"Diizinkan,Perbaikan,Dalam Proses,Ditolak,Semua"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B5">
+      <formula1>"namaIndex,noregisIndex,semuaIndex"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="B1:F6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="5" outlineLevelCol="5"/>
+  <cols>
+    <col min="2" max="2" width="24.2109375" customWidth="1"/>
+    <col min="3" max="3" width="20.5703125" customWidth="1"/>
+    <col min="4" max="4" width="29.2890625" customWidth="1"/>
+    <col min="5" max="5" width="23.703125" customWidth="1"/>
+    <col min="6" max="6" width="33.984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:6">
+      <c r="B1" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="2" spans="2:5">
+      <c r="B2" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" ht="15.6" spans="2:5">
+      <c r="B3" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" ht="15.6" spans="2:5">
+      <c r="B4" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5">
+      <c r="B5" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="4:5">
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B5">
+      <formula1>"namaCari,noregisCari,semuaCari"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5215,7 +5506,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="46" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -5278,7 +5569,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="46" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -5349,192 +5640,192 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="49" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="C1" s="49" t="s">
         <v>54</v>
       </c>
-      <c r="D1" s="46" t="s">
+      <c r="D1" s="49" t="s">
         <v>55</v>
       </c>
-      <c r="E1" s="46" t="s">
+      <c r="E1" s="49" t="s">
         <v>56</v>
       </c>
-      <c r="F1" s="46" t="s">
+      <c r="F1" s="49" t="s">
         <v>57</v>
       </c>
-      <c r="G1" s="46" t="s">
+      <c r="G1" s="49" t="s">
         <v>58</v>
       </c>
-      <c r="H1" s="50" t="s">
+      <c r="H1" s="53" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="34">
+      <c r="A2" s="37">
         <v>2</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="D2" s="8">
+      <c r="D2" s="11">
         <v>50120</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="H2" s="17" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="34"/>
-      <c r="B3" s="8" t="s">
+      <c r="A3" s="37"/>
+      <c r="B3" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="11">
         <v>50120</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="H3" s="17" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="34"/>
-      <c r="B4" s="8" t="s">
+      <c r="A4" s="37"/>
+      <c r="B4" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="11">
         <v>50120</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="H4" s="14" t="s">
+      <c r="H4" s="17" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="34"/>
-      <c r="B5" s="8" t="s">
+      <c r="A5" s="37"/>
+      <c r="B5" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="11">
         <v>50120</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="H5" s="14" t="s">
+      <c r="H5" s="17" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="34"/>
-      <c r="B6" s="8" t="s">
+      <c r="A6" s="37"/>
+      <c r="B6" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="11">
         <v>50120</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="G6" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="H6" s="14" t="s">
+      <c r="H6" s="17" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="7" ht="14.75" spans="1:8">
-      <c r="A7" s="35"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="8">
+      <c r="A7" s="38"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="11">
         <v>50120</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="G7" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="H7" s="37" t="s">
+      <c r="H7" s="40" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="11" ht="14.75"/>
     <row r="12" spans="1:1">
-      <c r="A12" s="47" t="s">
+      <c r="A12" s="50" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="48" t="s">
+      <c r="A13" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="49" t="s">
+      <c r="B13" s="52" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" s="8">
+      <c r="A14" s="11">
         <v>14</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="11" t="s">
         <v>27</v>
       </c>
     </row>
@@ -5569,7 +5860,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="46" t="s">
         <v>70</v>
       </c>
       <c r="B1" t="s">
@@ -5604,7 +5895,7 @@
       <c r="C2" t="s">
         <v>78</v>
       </c>
-      <c r="D2" s="44">
+      <c r="D2" s="47">
         <v>3434</v>
       </c>
       <c r="E2" t="s">
@@ -5627,7 +5918,7 @@
       <c r="C3" t="s">
         <v>83</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="11">
         <v>50120</v>
       </c>
       <c r="E3" t="s">
@@ -5644,7 +5935,7 @@
       <c r="C4" t="s">
         <v>83</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="11">
         <v>50120</v>
       </c>
       <c r="E4" t="s">
@@ -5661,7 +5952,7 @@
       <c r="C5" t="s">
         <v>83</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="11">
         <v>50120</v>
       </c>
       <c r="E5" t="s">
@@ -5712,248 +6003,248 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="42" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="31" t="s">
         <v>88</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="D1" s="31" t="s">
         <v>89</v>
       </c>
-      <c r="E1" s="28" t="s">
+      <c r="E1" s="31" t="s">
         <v>90</v>
       </c>
-      <c r="F1" s="28" t="s">
+      <c r="F1" s="31" t="s">
         <v>91</v>
       </c>
-      <c r="G1" s="28" t="s">
+      <c r="G1" s="31" t="s">
         <v>92</v>
       </c>
-      <c r="H1" s="28" t="s">
+      <c r="H1" s="31" t="s">
         <v>93</v>
       </c>
-      <c r="I1" s="28" t="s">
+      <c r="I1" s="31" t="s">
         <v>94</v>
       </c>
-      <c r="J1" s="28" t="s">
+      <c r="J1" s="31" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="39">
+      <c r="A2" s="42">
         <v>5</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="C2" s="40" t="s">
+      <c r="C2" s="43" t="s">
         <v>97</v>
       </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="40" t="s">
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="43" t="s">
         <v>98</v>
       </c>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="8"/>
-      <c r="B3" s="8" t="s">
+      <c r="A3" s="11"/>
+      <c r="B3" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="C3" s="40" t="s">
+      <c r="C3" s="43" t="s">
         <v>78</v>
       </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="40" t="s">
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="43" t="s">
         <v>98</v>
       </c>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="8"/>
-      <c r="B4" s="8" t="s">
+      <c r="A4" s="11"/>
+      <c r="B4" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="C4" s="40" t="s">
+      <c r="C4" s="43" t="s">
         <v>99</v>
       </c>
-      <c r="D4" s="40">
+      <c r="D4" s="43">
         <v>3460</v>
       </c>
-      <c r="E4" s="40" t="s">
+      <c r="E4" s="43" t="s">
         <v>100</v>
       </c>
-      <c r="F4" s="40" t="s">
+      <c r="F4" s="43" t="s">
         <v>101</v>
       </c>
-      <c r="G4" s="8"/>
-      <c r="H4" s="40" t="s">
+      <c r="G4" s="11"/>
+      <c r="H4" s="43" t="s">
         <v>98</v>
       </c>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="8"/>
-      <c r="B5" s="8" t="s">
+      <c r="A5" s="11"/>
+      <c r="B5" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="C5" s="40" t="s">
+      <c r="C5" s="43" t="s">
         <v>99</v>
       </c>
-      <c r="D5" s="40">
+      <c r="D5" s="43">
         <v>123</v>
       </c>
-      <c r="E5" s="40" t="s">
+      <c r="E5" s="43" t="s">
         <v>78</v>
       </c>
-      <c r="F5" s="40" t="s">
+      <c r="F5" s="43" t="s">
         <v>102</v>
       </c>
-      <c r="G5" s="40" t="s">
+      <c r="G5" s="43" t="s">
         <v>103</v>
       </c>
-      <c r="H5" s="40" t="s">
+      <c r="H5" s="43" t="s">
         <v>104</v>
       </c>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="8"/>
-      <c r="B6" s="8" t="s">
+      <c r="A6" s="11"/>
+      <c r="B6" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="8"/>
-      <c r="B7" s="8" t="s">
+      <c r="A7" s="11"/>
+      <c r="B7" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
+      <c r="A8" s="11"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
+      <c r="A9" s="11"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
+      <c r="A10" s="11"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="8"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
+      <c r="A11" s="11"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="8"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
+      <c r="A12" s="11"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="8"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
+      <c r="A13" s="11"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
+      <c r="A14" s="11"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11"/>
     </row>
     <row r="16" ht="14.75"/>
     <row r="17" ht="14.75" spans="1:2">
       <c r="A17" t="s">
         <v>105</v>
       </c>
-      <c r="B17" s="41"/>
+      <c r="B17" s="44"/>
     </row>
     <row r="18" ht="14.75" spans="1:2">
       <c r="A18" t="s">
         <v>106</v>
       </c>
-      <c r="B18" s="42"/>
+      <c r="B18" s="45"/>
     </row>
   </sheetData>
   <dataValidations count="2">
@@ -6019,7 +6310,7 @@
       <c r="E2">
         <v>1</v>
       </c>
-      <c r="F2" s="38" t="s">
+      <c r="F2" s="41" t="s">
         <v>113</v>
       </c>
       <c r="G2" t="s">

</xml_diff>